<commit_message>
analysis for pilot 2.1-2.3, power analysis for final data collection
</commit_message>
<xml_diff>
--- a/data/FYP_data_pilot_children_2.xlsx
+++ b/data/FYP_data_pilot_children_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marianna\Desktop\Dropbox\Stanford\projects\FYP structural blocking\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74B43FC9-6A68-43EA-96C6-B9E14F70BFB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{540F637D-7FC8-41DF-9FD9-B9211C68ED77}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="13970" windowHeight="9140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="pilot" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="122">
   <si>
     <t>gender</t>
   </si>
@@ -395,6 +395,12 @@
   </si>
   <si>
     <t>fc_expl_indiv_size_expl</t>
+  </si>
+  <si>
+    <t>ba815</t>
+  </si>
+  <si>
+    <t>FYP_20190410_01</t>
   </si>
 </sst>
 </file>
@@ -955,7 +961,7 @@
   <dimension ref="A1:AM24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -2789,6 +2795,21 @@
       </c>
     </row>
     <row r="24" spans="1:37" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>121</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" s="2">
+        <v>43565</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" t="s">
+        <v>120</v>
+      </c>
       <c r="F24">
         <v>5</v>
       </c>
@@ -2803,6 +2824,54 @@
       </c>
       <c r="J24" t="s">
         <v>107</v>
+      </c>
+      <c r="K24" t="s">
+        <v>42</v>
+      </c>
+      <c r="L24" t="s">
+        <v>42</v>
+      </c>
+      <c r="M24" t="s">
+        <v>42</v>
+      </c>
+      <c r="N24" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="4">
+        <v>5.4712328767123291</v>
+      </c>
+      <c r="P24" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>44</v>
+      </c>
+      <c r="R24" t="s">
+        <v>46</v>
+      </c>
+      <c r="S24" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" t="s">
+        <v>45</v>
+      </c>
+      <c r="U24" t="s">
+        <v>48</v>
+      </c>
+      <c r="W24" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK24" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2821,7 +2890,7 @@
   <dimension ref="A1:T10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>